<commit_message>
Niinkuin aiemmin ajateltu, muunnokset APIn tuomilla tiedoilla ennen power BI:tä ovat aivan turhia, koska data ei ole enään hirveen käytettävässä muodossa, muovattu siis esim moving time että antaa vain sekuntteina ja Power BI:ssä muunnos haluttuun muotoon
</commit_message>
<xml_diff>
--- a/Aktiviteetit/Vuosi_2025/Aktiviteetit_Heinäkuu.xlsx
+++ b/Aktiviteetit/Vuosi_2025/Aktiviteetit_Heinäkuu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,16 +478,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lunch Run</t>
+          <t>Intervallit</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>01:18:08</t>
-        </is>
+        <v>11.05</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3267</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -496,34 +494,32 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-09T12:24:49Z</t>
+          <t>2025-07-10T11:46:41Z</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>04:56</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2.561</v>
+        <v>3.383</v>
       </c>
       <c r="H2" t="n">
-        <v>139.5</v>
+        <v>158.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Säbä</t>
+          <t>Lunch Run</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.41</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>01:38:20</t>
-        </is>
+        <v>12</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4688</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -532,34 +528,32 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-08T19:33:57Z</t>
+          <t>2025-07-09T12:24:49Z</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.086</v>
+        <v>2.561</v>
       </c>
       <c r="H3" t="n">
-        <v>131.2</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Night Run</t>
+          <t>Säbä</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>01:01:06</t>
-        </is>
+        <v>6.41</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5900</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -568,34 +562,32 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-07T21:57:25Z</t>
+          <t>2025-07-08T19:33:57Z</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.479</v>
+        <v>1.086</v>
       </c>
       <c r="H4" t="n">
-        <v>138.6</v>
+        <v>131.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afternoon Run</t>
+          <t>Night Run</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.27</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>02:10:07</t>
-        </is>
+        <v>9.09</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3666</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -604,34 +596,32 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-05T16:17:54Z</t>
+          <t>2025-07-07T21:57:25Z</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>06:43</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2.724</v>
+        <v>2.479</v>
       </c>
       <c r="H5" t="n">
-        <v>145.7</v>
+        <v>138.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Vetoja</t>
+          <t>Afternoon Run</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.06</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>00:40:04</t>
-        </is>
+        <v>21.27</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7807</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -640,34 +630,32 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-03T20:37:43Z</t>
+          <t>2025-07-05T16:17:54Z</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>05:41</t>
+          <t>06:07</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2.938</v>
+        <v>2.724</v>
       </c>
       <c r="H6" t="n">
-        <v>153.8</v>
+        <v>145.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Morning Run</t>
+          <t>Vetoja</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10.65</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>01:11:48</t>
-        </is>
+        <v>7.06</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2404</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -676,34 +664,32 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-02T10:27:49Z</t>
+          <t>2025-07-03T20:37:43Z</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>06:45</t>
+          <t>05:41</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2.471</v>
+        <v>2.938</v>
       </c>
       <c r="H7" t="n">
-        <v>135</v>
+        <v>153.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Säbä</t>
+          <t>Morning Run</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.03</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>01:18:34</t>
-        </is>
+        <v>10.65</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4308</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -712,54 +698,86 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-01T20:42:49Z</t>
+          <t>2025-07-02T10:27:49Z</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1.067</v>
+        <v>2.471</v>
       </c>
       <c r="H8" t="n">
-        <v>142.1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Säbä</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4714</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-07-01T20:42:49Z</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1.067</v>
+      </c>
+      <c r="H9" t="n">
+        <v>142.1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Alkulämpöfutis</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>1.4</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>00:12:40</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Run</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="C10" t="n">
+        <v>760</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>2025-07-01T20:24:46Z</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>09:03</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>1.839</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
         <v>135.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pitää tarkistella tuota unix aikaa kun haetaan aktiviteetit, siinä käy virhe jos aktiviteetti alkanu ysin jälkeen, eli ongelma UTC ja UTC +3 välillä
</commit_message>
<xml_diff>
--- a/Aktiviteetit/Vuosi_2025/Aktiviteetit_Heinäkuu.xlsx
+++ b/Aktiviteetit/Vuosi_2025/Aktiviteetit_Heinäkuu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,14 +478,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Intervallit</t>
+          <t>Morning Run</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.05</v>
+        <v>9.31</v>
       </c>
       <c r="C2" t="n">
-        <v>3267</v>
+        <v>3983</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -494,32 +494,32 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-10T11:46:41Z</t>
+          <t>2025-07-14T09:56:26Z</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>04:56</t>
+          <t>07:08</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>3.383</v>
+        <v>2.339</v>
       </c>
       <c r="H2" t="n">
-        <v>158.5</v>
+        <v>140.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lunch Run</t>
+          <t>Afternoon Run</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>18.41</v>
       </c>
       <c r="C3" t="n">
-        <v>4688</v>
+        <v>5523</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -528,32 +528,32 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-09T12:24:49Z</t>
+          <t>2025-07-12T16:48:18Z</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>05:00</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2.561</v>
+        <v>3.334</v>
       </c>
       <c r="H3" t="n">
-        <v>139.5</v>
+        <v>168.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Säbä</t>
+          <t>Intervallit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.41</v>
+        <v>11.05</v>
       </c>
       <c r="C4" t="n">
-        <v>5900</v>
+        <v>3267</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -562,32 +562,32 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-08T19:33:57Z</t>
+          <t>2025-07-10T11:46:41Z</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>04:56</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.086</v>
+        <v>3.383</v>
       </c>
       <c r="H4" t="n">
-        <v>131.2</v>
+        <v>158.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Night Run</t>
+          <t>Lunch Run</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.09</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>3666</v>
+        <v>4688</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -596,32 +596,32 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-07T21:57:25Z</t>
+          <t>2025-07-09T12:24:49Z</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2.479</v>
+        <v>2.561</v>
       </c>
       <c r="H5" t="n">
-        <v>138.6</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afternoon Run</t>
+          <t>Säbä</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.27</v>
+        <v>6.41</v>
       </c>
       <c r="C6" t="n">
-        <v>7807</v>
+        <v>5900</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -630,32 +630,32 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-05T16:17:54Z</t>
+          <t>2025-07-08T19:33:57Z</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2.724</v>
+        <v>1.086</v>
       </c>
       <c r="H6" t="n">
-        <v>145.7</v>
+        <v>131.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Vetoja</t>
+          <t>Night Run</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.06</v>
+        <v>9.09</v>
       </c>
       <c r="C7" t="n">
-        <v>2404</v>
+        <v>3666</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -664,32 +664,32 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-03T20:37:43Z</t>
+          <t>2025-07-07T21:57:25Z</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>05:41</t>
+          <t>06:43</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2.938</v>
+        <v>2.479</v>
       </c>
       <c r="H7" t="n">
-        <v>153.8</v>
+        <v>138.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Morning Run</t>
+          <t>Afternoon Run</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10.65</v>
+        <v>21.27</v>
       </c>
       <c r="C8" t="n">
-        <v>4308</v>
+        <v>7807</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -698,32 +698,32 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-02T10:27:49Z</t>
+          <t>2025-07-05T16:17:54Z</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>06:45</t>
+          <t>06:07</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2.471</v>
+        <v>2.724</v>
       </c>
       <c r="H8" t="n">
-        <v>135</v>
+        <v>145.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Säbä</t>
+          <t>Vetoja</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.03</v>
+        <v>7.06</v>
       </c>
       <c r="C9" t="n">
-        <v>4714</v>
+        <v>2404</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -732,52 +732,120 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-01T20:42:49Z</t>
+          <t>2025-07-03T20:37:43Z</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>05:41</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1.067</v>
+        <v>2.938</v>
       </c>
       <c r="H9" t="n">
-        <v>142.1</v>
+        <v>153.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Morning Run</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4308</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-07-02T10:27:49Z</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>06:45</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>2.471</v>
+      </c>
+      <c r="H10" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Säbä</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4714</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-07-01T20:42:49Z</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1.067</v>
+      </c>
+      <c r="H11" t="n">
+        <v>142.1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>Alkulämpöfutis</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B12" t="n">
         <v>1.4</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C12" t="n">
         <v>760</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Run</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>2025-07-01T20:24:46Z</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>09:03</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="G12" t="n">
         <v>1.839</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H12" t="n">
         <v>135.1</v>
       </c>
     </row>

</xml_diff>